<commit_message>
domestication task complete in 30 mins look at me go
</commit_message>
<xml_diff>
--- a/data/seasonality.xlsx
+++ b/data/seasonality.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacks\Documents\GitHub\Zooarch_Exercise_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED559CB-EF4F-48B4-A94E-F8A6358CC4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A4FACA-C34D-40E7-9BCA-11E0231473E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36BCB45D-7D12-D94B-8256-73B51F003CAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36BCB45D-7D12-D94B-8256-73B51F003CAB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Svaerborg" sheetId="8" r:id="rId2"/>
+    <sheet name="Graph" sheetId="12" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Svaerborg" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Svaerborg 1 fused</t>
   </si>
@@ -47,6 +51,15 @@
   </si>
   <si>
     <t>Bin</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Fused</t>
+  </si>
+  <si>
+    <t>Unfused</t>
   </si>
 </sst>
 </file>
@@ -94,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -113,11 +126,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -137,6 +159,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,6 +178,1159 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Ringkloster</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Fused</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Graph!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graph!$B$2:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C0D6-40E2-8AA5-1701AAA5F2BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Unfused</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Graph!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graph!$C$2:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C0D6-40E2-8AA5-1701AAA5F2BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="288992480"/>
+        <c:axId val="812784208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="288992480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>SLC mm</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="812784208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="812784208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="288992480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Svaerborg</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.9413408238581182E-2"/>
+          <c:y val="0.15999071884075328"/>
+          <c:w val="0.85536897309088733"/>
+          <c:h val="0.66412831951139184"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Fused</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Svaerborg!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Svaerborg!$B$2:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-517C-4CFF-A751-9B6257A43D70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Unfused</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Svaerborg!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Svaerborg!$C$2:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-517C-4CFF-A751-9B6257A43D70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="682414224"/>
+        <c:axId val="681184224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="682414224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>SLC (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="681184224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="681184224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.4876660341555973E-3"/>
+              <c:y val="0.39085715996527048"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="682414224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.86318845343573036"/>
+          <c:y val="0.3570515852818778"/>
+          <c:w val="9.6963349220816092E-2"/>
+          <c:h val="0.1375126493218766"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -737,6 +1913,85 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C77152A6-2957-42CE-B856-DE3388F4E0A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70E6E2E9-779B-4E1C-B74B-99DF0FA0DE1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1073,11 +2328,368 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE66D17-5C3C-437C-9CB7-F0537A1CAB5A}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="6">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="6">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="6">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="6">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="6">
+        <v>17</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="6">
+        <v>19</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="6">
+        <v>20</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="6">
+        <v>21</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="6">
+        <v>22</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="6">
+        <v>23</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6">
+        <v>24</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6">
+        <v>25</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="6">
+        <v>26</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="6">
+        <v>27</v>
+      </c>
+      <c r="B20" s="7">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="6">
+        <v>28</v>
+      </c>
+      <c r="B21" s="7">
+        <v>2</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="6">
+        <v>29</v>
+      </c>
+      <c r="B22" s="7">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="6">
+        <v>30</v>
+      </c>
+      <c r="B23" s="7">
+        <v>6</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="6">
+        <v>31</v>
+      </c>
+      <c r="B24" s="7">
+        <v>8</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="6">
+        <v>32</v>
+      </c>
+      <c r="B25" s="7">
+        <v>14</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="6">
+        <v>33</v>
+      </c>
+      <c r="B26" s="7">
+        <v>10</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="6">
+        <v>34</v>
+      </c>
+      <c r="B27" s="7">
+        <v>7</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6">
+        <v>35</v>
+      </c>
+      <c r="B28" s="7">
+        <v>4</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="6">
+        <v>36</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="6">
+        <v>37</v>
+      </c>
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A30">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626C5DFA-CA8A-B140-956D-3E8E9051D890}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1088,7 +2700,7 @@
     <col min="4" max="4" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1958,7 +3570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E0B889-58A2-0E40-93AB-633F7E5580AC}">
   <dimension ref="A1:C30"/>
   <sheetViews>

</xml_diff>